<commit_message>
Use from XSD converted XML-Serializer class MusicalNoteList instead for parsing the embedded PianoKeyToFrequency.xml instead using hand written handling of the XML parsed items.
</commit_message>
<xml_diff>
--- a/FrequencyToPianoKey.xlsx
+++ b/FrequencyToPianoKey.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leuze-my.sharepoint.com/personal/mkaul_leuze_com/Documents/Projects/VoiceControl/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkaul\OneDrive - Leuze electronic GmbH + Co. KG\Projects\VoiceControl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{216F8E9C-1F37-4FEF-9C05-7E9637DBFF6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{59DF9A58-8A10-4F71-AADA-A1DFAF90A81E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -561,7 +560,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -596,7 +595,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -613,49 +612,54 @@
 
 <file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
 <MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="xmlns:ns1='http://www.exampleURI.com/Schema1'">
-  <Schema ID="Schema1" Namespace="http://www.exampleURI.com/Schema1">
+  <Schema ID="Schema3" Namespace="http://www.exampleURI.com/Schema1">
     <xs:schema xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns="PianoKeyToFrequency" xmlns:s1="http://www.exampleURI.com/Schema1" targetNamespace="http://www.exampleURI.com/Schema1">
-      <xs:element name="Root" type="xs:string"/>
-      <xs:element name="MusicNoteList" type="s1:MusicNoteList"/>
-      <xs:complexType name="MusicNoteList">
+      <xs:element name="MusicalNote" type="s1:MusicalNote"/>
+      <xs:complexType name="MusicalNote">
+        <xs:annotation>
+          <xs:documentation>Defines one musical-note represented by frequency, names and piano-key number.</xs:documentation>
+        </xs:annotation>
         <xs:sequence>
-          <xs:element name="MusicNote" minOccurs="0" maxOccurs="unbounded">
-            <xs:complexType>
-              <xs:sequence>
-                <xs:element name="Frequency" type="xs:float" minOccurs="1" maxOccurs="1"/>
-                <xs:element name="NotationEng" type="xs:string" minOccurs="1" maxOccurs="1"/>
-                <xs:element name="NotationGer" type="xs:string" minOccurs="1" maxOccurs="1"/>
-                <xs:element name="NotationGerSimple" type="xs:string" minOccurs="1" maxOccurs="1"/>
-                <xs:element name="PianoKey" type="xs:short" minOccurs="1" maxOccurs="1"/>
-              </xs:sequence>
-            </xs:complexType>
-          </xs:element>
+          <xs:element name="Frequency" type="xs:float" minOccurs="1" maxOccurs="1"/>
+          <xs:element name="NotationEng" type="xs:string" minOccurs="1" maxOccurs="1"/>
+          <xs:element name="NotationGer" type="xs:string" minOccurs="1" maxOccurs="1"/>
+          <xs:element name="NotationGerSimple" type="xs:string" minOccurs="1" maxOccurs="1"/>
+          <xs:element name="PianoKey" type="xs:short" minOccurs="1" maxOccurs="1"/>
+        </xs:sequence>
+      </xs:complexType>
+      <xs:element name="MusicalNoteList" type="s1:MusicalNoteList"/>
+      <xs:complexType name="MusicalNoteList">
+        <xs:annotation>
+          <xs:documentation>Container musical-note definitions.</xs:documentation>
+        </xs:annotation>
+        <xs:sequence>
+          <xs:element name="MusicalNote" type="s1:MusicalNote" minOccurs="0" maxOccurs="unbounded"/>
         </xs:sequence>
       </xs:complexType>
     </xs:schema>
   </Schema>
-  <Map ID="1" Name="MusicNoteList_Map" RootElement="MusicNoteList" SchemaID="Schema1" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
+  <Map ID="3" Name="MusicalNoteList_Zuordnung" RootElement="MusicalNoteList" SchemaID="Schema3" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{62575136-0D32-47D3-9D6C-17613569893D}" name="Table4" displayName="Table4" ref="A1:E89" tableType="xml" totalsRowShown="0">
-  <autoFilter ref="A1:E89" xr:uid="{64C7C463-4061-4FAB-98D0-722BCBE47C9D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:E89" tableType="xml" totalsRowShown="0">
+  <autoFilter ref="A1:E89"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D486B6CA-3116-41D4-A1DE-95A2615B2DC2}" uniqueName="PianoKey" name="Tastennummer">
-      <xmlColumnPr mapId="1" xpath="/ns1:MusicNoteList/MusicNote/PianoKey" xmlDataType="short"/>
+    <tableColumn id="1" uniqueName="PianoKey" name="Tastennummer">
+      <xmlColumnPr mapId="3" xpath="/ns1:MusicalNoteList/MusicalNote/PianoKey" xmlDataType="short"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{D780A2FB-41EA-44B2-905B-DBC2C38D04D7}" uniqueName="NotationEng" name="Notation (englisch)">
-      <xmlColumnPr mapId="1" xpath="/ns1:MusicNoteList/MusicNote/NotationEng" xmlDataType="string"/>
+    <tableColumn id="2" uniqueName="NotationEng" name="Notation (englisch)">
+      <xmlColumnPr mapId="3" xpath="/ns1:MusicalNoteList/MusicalNote/NotationEng" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{A24F9266-A10C-4CCE-9413-6C5753BBAC1D}" uniqueName="NotationGer" name="Notation (deutsch)">
-      <xmlColumnPr mapId="1" xpath="/ns1:MusicNoteList/MusicNote/NotationGer" xmlDataType="string"/>
+    <tableColumn id="3" uniqueName="NotationGer" name="Notation (deutsch)">
+      <xmlColumnPr mapId="3" xpath="/ns1:MusicalNoteList/MusicalNote/NotationGer" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DBBDA6F4-43FF-44D9-AF14-EB6DB315A397}" uniqueName="NotationGerSimple" name="Notation (deutsch) einfach">
-      <xmlColumnPr mapId="1" xpath="/ns1:MusicNoteList/MusicNote/NotationGerSimple" xmlDataType="string"/>
+    <tableColumn id="4" uniqueName="NotationGerSimple" name="Notation (deutsch) einfach">
+      <xmlColumnPr mapId="3" xpath="/ns1:MusicalNoteList/MusicalNote/NotationGerSimple" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{3A9151FD-0802-429F-B077-F4E8AF3B9AA6}" uniqueName="Frequency" name="Frequenz in Hertz">
-      <xmlColumnPr mapId="1" xpath="/ns1:MusicNoteList/MusicNote/Frequency" xmlDataType="float"/>
+    <tableColumn id="5" uniqueName="Frequency" name="Frequenz in Hertz">
+      <xmlColumnPr mapId="3" xpath="/ns1:MusicalNoteList/MusicalNote/Frequency" xmlDataType="float"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -958,14 +962,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A19EEAF6-370F-4F45-A6E5-A2E46C0F2C65}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="2" width="20.140625" customWidth="1"/>

</xml_diff>